<commit_message>
V9.0 Wprowadzanie swojego nicku
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,7 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -475,7 +471,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +480,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>maziar</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -494,11 +490,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -507,7 +503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maksssssssssss</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,11 +513,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -530,32 +526,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>485</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -563,22 +555,18 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>540</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -586,11 +574,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
@@ -604,16 +592,16 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -627,16 +615,16 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -650,16 +638,16 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -673,16 +661,16 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>485</v>
       </c>
     </row>
     <row r="12">
@@ -696,16 +684,16 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
+        <v>540</v>
       </c>
     </row>
     <row r="13">
@@ -719,7 +707,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -728,7 +716,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14">
@@ -742,16 +730,16 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -765,16 +753,16 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -788,16 +776,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -811,16 +799,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -834,16 +822,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -857,16 +845,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -880,15 +868,153 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>Wielkopolskie</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Lubuskie</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="E25" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Kujawsko-Pomorskie</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V10.0 Zmienna rozdzielczość, ujodnlocenie nazw na polskie poza tytułem
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Nazwa</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Level</t>
+          <t>Poziom</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Voivodeship</t>
+          <t>Województwo</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Points</t>
+          <t>Punkty</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,11 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -467,11 +471,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -480,12 +484,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>maziar</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -494,7 +498,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -503,21 +507,21 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Maksssssssssss</t>
+          <t>kk</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -526,12 +530,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -540,17 +544,21 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>hh</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -559,26 +567,30 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ii</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -587,7 +599,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -597,11 +609,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -610,21 +622,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -633,12 +645,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -647,7 +659,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -656,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -666,11 +678,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>485</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -679,7 +691,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>jjj</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -689,11 +701,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>540</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
@@ -702,7 +714,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>;;</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -712,11 +724,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -725,21 +737,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
@@ -748,67 +760,59 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
@@ -817,21 +821,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>lala</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
@@ -840,21 +844,21 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>kuba</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -863,21 +867,21 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
@@ -886,7 +890,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -896,11 +900,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -909,7 +913,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -923,7 +927,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23">
@@ -932,7 +936,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -942,11 +946,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -955,7 +959,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -965,11 +969,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
@@ -978,7 +982,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -988,11 +992,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -1001,7 +1005,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1011,10 +1015,619 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Łódzkie</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Karolcio</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Wielkopolskie</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Dolnośląskie</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>maziar</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Podlaskie</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Maksssssssssss</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Łódzkie</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Podlaskie</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Podlaskie</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Dolnośląskie</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Dolnośląskie</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Dolnośląskie</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Podlaskie</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Wszystkie</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Wszystkie</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Wielkopolskie</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Lubuskie</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="E52" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Kujawsko-Pomorskie</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V11.0 Kolejne jakieś zmiany
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
@@ -484,21 +484,21 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>kk</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,11 +517,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -530,7 +530,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -553,12 +553,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>hh</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -576,21 +576,21 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ii</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -599,21 +599,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -622,7 +622,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,11 +632,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -645,7 +645,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -668,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,11 +678,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -691,7 +691,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>jjj</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -701,11 +701,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -714,7 +714,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>;;</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -724,11 +724,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14">
@@ -737,21 +737,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -760,28 +760,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -800,7 +804,11 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -808,11 +816,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
@@ -821,7 +829,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>lala</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -831,11 +839,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
@@ -844,7 +852,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>kuba</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -854,11 +862,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -867,7 +875,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>jjj</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -881,7 +889,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
@@ -890,7 +898,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>;;</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -900,11 +908,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
@@ -913,7 +921,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -923,11 +931,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
@@ -946,22 +954,18 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -969,22 +973,18 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -992,11 +992,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>lala</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1015,11 +1015,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kuba</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1038,11 +1038,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Karolcio</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1061,18 +1061,22 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1080,11 +1084,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
@@ -1093,21 +1097,21 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>maziar</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31">
@@ -1116,21 +1120,21 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Maksssssssssss</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
@@ -1144,23 +1148,27 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1168,18 +1176,22 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1187,11 +1199,11 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
@@ -1200,7 +1212,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1210,11 +1222,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -1223,44 +1235,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Karolcio</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38">
@@ -1269,21 +1277,21 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>maziar</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>485</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
@@ -1292,21 +1300,21 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maksssssssssss</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>540</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1315,67 +1323,59 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43">
@@ -1389,16 +1389,16 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
@@ -1412,16 +1412,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45">
@@ -1435,16 +1435,16 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46">
@@ -1458,16 +1458,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>485</v>
       </c>
     </row>
     <row r="47">
@@ -1481,16 +1481,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>13</v>
+        <v>540</v>
       </c>
     </row>
     <row r="48">
@@ -1509,11 +1509,11 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49">
@@ -1527,16 +1527,16 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
@@ -1550,16 +1550,16 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
@@ -1573,16 +1573,16 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -1596,16 +1596,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53">
@@ -1619,15 +1619,199 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Wielkopolskie</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Lubuskie</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
-      <c r="E53" t="n">
+      <c r="E60" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Kujawsko-Pomorskie</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V14.0 Wiekszość rozwiązana z wykorzystaniem klasy Game
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,23 +461,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>kkk</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>Lubelskie</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -486,7 +484,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>aaaaa</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -496,11 +494,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -509,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -519,11 +517,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
@@ -532,7 +530,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -542,11 +540,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -555,21 +553,21 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -578,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -588,11 +586,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -601,7 +599,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -611,11 +609,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -624,7 +622,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>ytg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -634,11 +632,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -647,21 +645,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kkk</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -670,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aaaaa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -680,11 +678,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>72</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -703,11 +701,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -726,11 +724,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
@@ -744,7 +742,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -753,7 +751,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -772,7 +770,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -795,11 +793,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>87</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -808,7 +806,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -818,11 +816,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -831,7 +829,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -841,11 +839,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>66</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
@@ -854,7 +852,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>hhh</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -864,11 +862,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>15</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
@@ -877,7 +875,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -887,11 +885,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21">
@@ -900,21 +898,21 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22">
@@ -923,7 +921,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -937,7 +935,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -946,7 +944,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -956,11 +954,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -969,7 +967,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -979,11 +977,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>15</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25">
@@ -992,7 +990,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1002,11 +1000,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>60</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26">
@@ -1015,21 +1013,21 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>22</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27">
@@ -1038,7 +1036,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>hhh</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1048,11 +1046,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
@@ -1061,7 +1059,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1075,7 +1073,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
@@ -1084,21 +1082,21 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -1107,7 +1105,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1117,11 +1115,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31">
@@ -1130,7 +1128,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1144,7 +1142,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
@@ -1153,12 +1151,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1167,7 +1165,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
@@ -1176,21 +1174,21 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34">
@@ -1199,21 +1197,21 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35">
@@ -1232,11 +1230,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -1278,11 +1276,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
@@ -1291,7 +1289,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>jjj</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1301,11 +1299,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -1314,7 +1312,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>;;</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1324,11 +1322,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
@@ -1337,21 +1335,21 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -1365,23 +1363,27 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1400,7 +1402,11 @@
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1408,11 +1414,11 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44">
@@ -1421,7 +1427,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>lala</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1431,11 +1437,11 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
@@ -1444,7 +1450,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>kuba</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1454,11 +1460,11 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46">
@@ -1467,7 +1473,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>jjj</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1481,7 +1487,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47">
@@ -1490,7 +1496,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>;;</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1500,11 +1506,11 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
@@ -1513,7 +1519,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1523,11 +1529,11 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49">
@@ -1546,22 +1552,18 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1569,22 +1571,18 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1592,11 +1590,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52">
@@ -1605,7 +1603,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>lala</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1615,11 +1613,11 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53">
@@ -1628,7 +1626,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kuba</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1638,11 +1636,11 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
@@ -1651,7 +1649,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Karolcio</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1661,18 +1659,22 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1680,11 +1682,11 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -1693,21 +1695,21 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>maziar</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57">
@@ -1716,21 +1718,21 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Maksssssssssss</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58">
@@ -1744,23 +1746,27 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1768,18 +1774,22 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1787,11 +1797,11 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61">
@@ -1800,7 +1810,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1810,11 +1820,11 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62">
@@ -1823,44 +1833,40 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Karolcio</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64">
@@ -1869,21 +1875,21 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>maziar</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>485</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
@@ -1892,21 +1898,21 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maksssssssssss</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>540</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -1915,67 +1921,59 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69">
@@ -1989,16 +1987,16 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="70">
@@ -2012,16 +2010,16 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71">
@@ -2035,16 +2033,16 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72">
@@ -2058,16 +2056,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>5</v>
+        <v>485</v>
       </c>
     </row>
     <row r="73">
@@ -2081,16 +2079,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>13</v>
+        <v>540</v>
       </c>
     </row>
     <row r="74">
@@ -2109,11 +2107,11 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75">
@@ -2127,16 +2125,16 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76">
@@ -2150,16 +2148,16 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -2173,16 +2171,16 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
@@ -2196,16 +2194,16 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
@@ -2219,15 +2217,199 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Pomorskie</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Easy</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Wielkopolskie</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Lubuskie</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
           <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
-      <c r="E79" t="n">
+      <c r="E86" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Kujawsko-Pomorskie</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V15.0 Wszystko z klasą Game, ale jeszcze bez skalowania w Game + lekkie optymalizacje kodu
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -494,11 +494,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,11 +517,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -530,7 +530,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -540,11 +540,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -553,12 +553,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>67</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -586,11 +586,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -599,21 +599,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>21</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
@@ -622,7 +622,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ytg</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,11 +632,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -645,21 +645,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>kkk</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>aaaaa</t>
+          <t>ytg</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,11 +678,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -691,21 +691,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kkk</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -714,7 +714,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aaaaa</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -724,11 +724,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -742,16 +742,16 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -770,11 +770,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -788,7 +788,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -839,11 +839,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -862,11 +862,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20">
@@ -885,11 +885,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
@@ -908,11 +908,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22">
@@ -931,11 +931,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
@@ -954,11 +954,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24">
@@ -977,11 +977,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>87</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
@@ -990,7 +990,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1000,11 +1000,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>66</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>hhh</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1046,11 +1046,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1069,11 +1069,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29">
@@ -1082,21 +1082,21 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>hhh</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1128,21 +1128,21 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32">
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33">
@@ -1184,11 +1184,11 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34">
@@ -1202,16 +1202,16 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1230,11 +1230,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36">
@@ -1243,21 +1243,21 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37">
@@ -1276,11 +1276,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
@@ -1299,11 +1299,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40">
@@ -1340,16 +1340,16 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
@@ -1363,16 +1363,16 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1395,7 +1395,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43">
@@ -1409,16 +1409,16 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1441,7 +1441,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45">
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>jjj</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1483,11 +1483,11 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>;;</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1506,11 +1506,11 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48">
@@ -1519,7 +1519,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>jjj</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1529,11 +1529,11 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>;;</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1556,14 +1556,18 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>aaa</t>
+        </is>
+      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1571,18 +1575,22 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1590,7 +1598,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -1601,11 +1609,7 @@
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>lala</t>
-        </is>
-      </c>
+      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1613,22 +1617,18 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>kuba</t>
-        </is>
-      </c>
+      <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1636,11 +1636,11 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>lala</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1659,11 +1659,11 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kuba</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1682,11 +1682,11 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59">
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60">
@@ -1801,7 +1801,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61">
@@ -1820,11 +1820,11 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Karolcio</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1843,18 +1843,22 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr"/>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1862,11 +1866,11 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64">
@@ -1875,44 +1879,40 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>maziar</t>
+          <t>Karolcio</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Maksssssssssss</t>
-        </is>
-      </c>
+      <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maziar</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1935,56 +1935,60 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="inlineStr"/>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Maksssssssssss</t>
+        </is>
+      </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1992,25 +1996,21 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>maks</t>
-        </is>
-      </c>
+      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2019,7 +2019,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="71">
@@ -2033,16 +2033,16 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72">
@@ -2056,16 +2056,16 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>485</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73">
@@ -2079,16 +2079,16 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>540</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74">
@@ -2107,11 +2107,11 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>15</v>
+        <v>485</v>
       </c>
     </row>
     <row r="75">
@@ -2125,16 +2125,16 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>8</v>
+        <v>540</v>
       </c>
     </row>
     <row r="76">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -2263,16 +2263,16 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -2286,16 +2286,16 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -2309,16 +2309,16 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84">
@@ -2337,11 +2337,11 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85">
@@ -2360,11 +2360,11 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86">
@@ -2383,11 +2383,11 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87">
@@ -2406,10 +2406,56 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
+          <t>Śląskie</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
           <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
-      <c r="E87" t="n">
+      <c r="E88" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Kujawsko-Pomorskie</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V15.1 Wszystko z klasą Game, ale jeszcze bez skalowania w Game + lekkie optymalizacje kodu
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>l</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,11 +471,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -484,7 +484,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>32</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,11 +517,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>29</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
@@ -530,7 +530,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
@@ -553,12 +553,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -586,11 +586,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8">
@@ -599,21 +599,21 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -622,7 +622,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,11 +632,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -645,7 +645,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>Karolcio</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -655,11 +655,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ytg</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,11 +678,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -691,21 +691,21 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>kkk</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -714,7 +714,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>aaaaa</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -724,22 +724,18 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -747,11 +743,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15">
@@ -760,21 +756,21 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kkk</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -806,7 +802,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -816,11 +812,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
@@ -829,7 +825,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -839,11 +835,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
@@ -852,7 +848,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -862,11 +858,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
@@ -875,7 +871,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -885,11 +881,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21">
@@ -898,7 +894,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -912,7 +908,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22">
@@ -921,7 +917,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -931,22 +927,18 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -954,11 +946,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
@@ -967,7 +959,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -977,11 +969,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25">
@@ -1000,22 +992,18 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1023,11 +1011,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27">
@@ -1036,7 +1024,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1046,11 +1034,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28">
@@ -1059,7 +1047,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1073,7 +1061,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29">
@@ -1082,7 +1070,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>hhh</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1092,11 +1080,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30">
@@ -1128,21 +1116,21 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>h</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32">
@@ -1151,7 +1139,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>aaa</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1161,7 +1149,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1179,16 +1167,16 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
@@ -1197,7 +1185,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1207,11 +1195,11 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
@@ -1220,7 +1208,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1230,11 +1218,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>60</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36">
@@ -1243,21 +1231,21 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
@@ -1266,7 +1254,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>;;</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1276,11 +1264,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38">
@@ -1289,7 +1277,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1299,11 +1287,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
@@ -1312,7 +1300,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>lala</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1322,11 +1310,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40">
@@ -1349,7 +1337,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41">
@@ -1358,7 +1346,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1368,11 +1356,11 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42">
@@ -1381,21 +1369,21 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43">
@@ -1404,21 +1392,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44">
@@ -1427,21 +1415,21 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45">
@@ -1460,11 +1448,11 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46">
@@ -1473,7 +1461,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1487,7 +1475,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47">
@@ -1506,11 +1494,11 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48">
@@ -1519,7 +1507,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>jjj</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1529,7 +1517,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -1542,7 +1530,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>;;</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1552,11 +1540,11 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50">
@@ -1565,7 +1553,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>aaa</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1575,22 +1563,18 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1598,18 +1582,22 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>wiki &lt;3</t>
+        </is>
+      </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1628,7 +1616,11 @@
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>jjj</t>
+        </is>
+      </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1636,11 +1628,11 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54">
@@ -1649,7 +1641,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>lala</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1659,11 +1651,11 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55">
@@ -1672,7 +1664,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>kuba</t>
+          <t>hhh</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1682,11 +1674,11 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56">
@@ -1695,21 +1687,21 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57">
@@ -1718,7 +1710,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aaaaa</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1728,11 +1720,11 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58">
@@ -1741,32 +1733,28 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1774,11 +1762,11 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60">
@@ -1787,7 +1775,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>kuba</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1797,7 +1785,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E60" t="n">
@@ -1820,11 +1808,11 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62">
@@ -1843,11 +1831,11 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63">
@@ -1866,11 +1854,11 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64">
@@ -1879,7 +1867,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Karolcio</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1889,30 +1877,34 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr"/>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66">
@@ -1921,12 +1913,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>maziar</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1935,7 +1927,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67">
@@ -1944,21 +1936,21 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Maksssssssssss</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68">
@@ -1972,23 +1964,27 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="inlineStr"/>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -2000,14 +1996,18 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Maks</t>
+        </is>
+      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -2015,11 +2015,11 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71">
@@ -2038,11 +2038,11 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72">
@@ -2061,11 +2061,11 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>maziar</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74">
@@ -2097,21 +2097,21 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maksssssssssss</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>485</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75">
@@ -2120,7 +2120,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2130,11 +2130,11 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>540</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2153,11 +2153,11 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -2166,21 +2166,21 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78">
@@ -2189,12 +2189,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
@@ -2212,21 +2212,21 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80">
@@ -2240,16 +2240,16 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81">
@@ -2258,21 +2258,21 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Pomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82">
@@ -2309,16 +2309,16 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
@@ -2327,21 +2327,21 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
@@ -2355,16 +2355,16 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86">
@@ -2378,16 +2378,16 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2406,11 +2406,11 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
@@ -2419,21 +2419,21 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -2447,16 +2447,39 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Pomorskie</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>18</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ytg</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Extreme</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Opolskie</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V17.0 poprawki mnożnika, poprawiona organizacja, estetyka kodu
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -457,7 +457,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -480,7 +480,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -503,11 +503,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>j</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -530,7 +530,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>'</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>testowańsko</t>
+          <t>'</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11111</t>
+          <t>testowańsko</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -586,11 +586,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8">
@@ -599,7 +599,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>11111</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -609,11 +609,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
@@ -622,7 +622,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -632,11 +632,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10">
@@ -645,7 +645,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -655,11 +655,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
@@ -668,7 +668,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -678,20 +678,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>l</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -701,25 +701,25 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>l</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -737,21 +737,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Easy</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -760,7 +760,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -770,11 +770,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16">
@@ -783,7 +783,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>testyyyyyyy</t>
+          <t>wiki &lt;3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -793,11 +793,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
@@ -806,21 +806,21 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>testyyyyyyy</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18">
@@ -829,21 +829,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>k</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
@@ -852,7 +852,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -862,30 +862,30 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Karolcio</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -894,11 +894,11 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>Karolcio</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -908,18 +908,22 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Wielkopolskie</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B22" t="inlineStr"/>
+        <v>19</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -927,20 +931,20 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>maks</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -950,41 +954,41 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B24" t="inlineStr"/>
+        <v>24</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>szymek</t>
-        </is>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -992,16 +996,16 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Kujawsko-Pomorskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1010,21 +1014,21 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1051,7 +1055,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>uj</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1061,34 +1065,30 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>szymek</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1107,30 +1107,30 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Kujawsko-Pomorskie</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1139,9 +1139,13 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" t="inlineStr"/>
+        <v>37</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1149,7 +1153,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1158,11 +1162,11 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1172,7 +1176,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Śląskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1181,13 +1185,9 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>h</t>
-        </is>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1204,11 +1204,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>pkstz</t>
+          <t>h</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1227,11 +1227,11 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>'</t>
+          <t>pkstz</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1241,41 +1241,45 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>aa</t>
+          <t>uj</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B38" t="inlineStr"/>
+        <v>30</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>maks</t>
+        </is>
+      </c>
       <c r="C38" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1283,11 +1287,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Śląskie</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39">
@@ -1296,7 +1300,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>hjk</t>
+          <t>'</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1306,11 +1310,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40">
@@ -1319,7 +1323,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>aa</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1329,11 +1333,11 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Wszystkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41">
@@ -1348,34 +1352,30 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Łódzkie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Maks</t>
-        </is>
-      </c>
+      <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Extreme</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Maks</t>
+          <t>hjk</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1394,11 +1394,11 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Zachodniopomorskie</t>
+          <t>Lubelskie</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="44">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>mak</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1417,20 +1417,20 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Wszystkie</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>iu</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1440,20 +1440,20 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Łódzkie</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1463,22 +1463,18 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Zachodniopomorskie</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>aaa</t>
-        </is>
-      </c>
+      <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
           <t>Extreme</t>
@@ -1490,7 +1486,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48">
@@ -1499,7 +1495,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>Maks</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1509,43 +1505,43 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Podlaskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>wiki &lt;3</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Easy</t>
+          <t>Extreme</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Lubelskie</t>
+          <t>Dolnośląskie</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>maks</t>
+          <t>mak</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1555,20 +1551,20 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Dolnośląskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>fg</t>
+          <t>;</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1578,11 +1574,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>